<commit_message>
Update Iter 7 Test Cases and test result for screenings
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 6/Iteration 6 Test Cases v3 Result.xlsx
+++ b/Test Cases/Iteration 6/Iteration 6 Test Cases v3 Result.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="162">
   <si>
     <t>No</t>
   </si>
@@ -413,13 +413,6 @@
     <t>Add Screening : Wrong Age Group</t>
   </si>
   <si>
-    <t>Age : 9
-Common illness:  Fever
-Recommended screening:  - 
-Demographic affected: Infant, Female, Male
-Regularity : 0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Error Message Shown (Infant cannot be above 1 years old) </t>
   </si>
   <si>
@@ -554,9 +547,6 @@
     <t>Type are sorted in alphatical order (A - Z)</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t xml:space="preserve">Click on the 'View Screenings' from the Screenings drop down list on the header  </t>
   </si>
   <si>
@@ -566,22 +556,7 @@
     <t>Verify that logged in user can access the view screenings tab</t>
   </si>
   <si>
-    <t>Redirect back to screening page, screening not shown</t>
-  </si>
-  <si>
     <t>Success Message shown, redirect to view screenings page</t>
-  </si>
-  <si>
-    <t>Demographic affected was female, female, male</t>
-  </si>
-  <si>
-    <t>No message to indicate screening updated</t>
-  </si>
-  <si>
-    <t>Illness for infant added</t>
-  </si>
-  <si>
-    <t>"Successfully added" and redirect to view screenings</t>
   </si>
   <si>
     <t xml:space="preserve">Access the URL: viewscreenings.html
@@ -667,8 +642,68 @@
 Regularity : 1 </t>
   </si>
   <si>
+    <t xml:space="preserve">Edit Screening (Type: Female) </t>
+  </si>
+  <si>
+    <t>Age : 1 month
+Common illness:  Hepatitis B
+Recommended screening:Hepatitis B-2nd Dose
+Demographic affected: Infant
+Regularity : 0</t>
+  </si>
+  <si>
+    <t>Age : 0 month
+Common illness:  Hepatitis B
+Recommended screening: Hepatitis B-1st Dose
+Demographic affected: Infant
+Regularity : 0</t>
+  </si>
+  <si>
+    <t>Able to access the link</t>
+  </si>
+  <si>
+    <t>Able to access the tab</t>
+  </si>
+  <si>
+    <t>ecf</t>
+  </si>
+  <si>
+    <t>Age : 25
+Common illness:  Fever
+Recommended screening:  - 
+Demographic affected: Infant
+Regularity : 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message shown (less than 24 months) </t>
+  </si>
+  <si>
+    <t>Illness for infant not added</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Age : 5
+      <t xml:space="preserve">Age : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Common illness:  Hand Foot Mouth Disease  
 Recommended screening:  Body Checkup
 Demographic affected: </t>
@@ -704,34 +739,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Regularity : 0</t>
+      <t>Regularity : 1</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Edit Screening (Type: Female) </t>
-  </si>
-  <si>
-    <t>Age : 1 month
-Common illness:  Hepatitis B
-Recommended screening:Hepatitis B-2nd Dose
-Demographic affected: Infant
-Regularity : 0</t>
-  </si>
-  <si>
-    <t>Age : 0 month
-Common illness:  Hepatitis B
-Recommended screening: Hepatitis B-1st Dose
-Demographic affected: Infant
-Regularity : 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -761,12 +786,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -781,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -789,14 +820,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -809,6 +840,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1802,7 +1842,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>24</v>
@@ -1959,7 +1999,7 @@
         <v>70</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2170,16 +2210,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2192,16 +2232,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -2214,16 +2254,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2236,16 +2276,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -3381,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3430,8 +3470,8 @@
       <c r="D2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>132</v>
+      <c r="E2" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
@@ -3454,7 +3494,7 @@
         <v>77</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>6</v>
@@ -3477,7 +3517,7 @@
         <v>77</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
@@ -3494,15 +3534,15 @@
         <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="10"/>
@@ -3520,9 +3560,11 @@
         <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
@@ -3538,12 +3580,14 @@
         <v>83</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3556,19 +3600,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>134</v>
+      <c r="E8" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -3588,10 +3632,10 @@
         <v>87</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -3611,7 +3655,7 @@
         <v>90</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>6</v>
@@ -3628,16 +3672,16 @@
         <v>91</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -3654,115 +3698,110 @@
         <v>84</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" ht="62" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+      <c r="A13" s="12">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" ht="62" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+      <c r="A14" s="12">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="62" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+      <c r="A15" s="12">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" ht="300" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+      <c r="A16" s="12">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="196.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="196.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="196.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
@@ -3772,13 +3811,13 @@
         <v>88</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>6</v>
@@ -3789,16 +3828,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>6</v>
@@ -3809,16 +3848,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>6</v>
@@ -3829,16 +3868,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>6</v>
@@ -3849,16 +3888,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>6</v>
@@ -3869,16 +3908,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>6</v>
@@ -3888,117 +3927,107 @@
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>113</v>
+      <c r="B25" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>116</v>
+      <c r="B26" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>117</v>
+      <c r="B27" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>118</v>
+      <c r="B28" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>6</v>
@@ -4009,40 +4038,38 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>127</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>143</v>
+      <c r="B31" s="12" t="s">
+        <v>136</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="F31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update iter 6 result
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 6/Iteration 6 Test Cases v3 Result.xlsx
+++ b/Test Cases/Iteration 6/Iteration 6 Test Cases v3 Result.xlsx
@@ -3421,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated Test Cases for Iter 6&7 (Screenings/Bootstrap) + Bootstrap Test files (sequence)
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 6/Iteration 6 Test Cases v3 Result.xlsx
+++ b/Test Cases/Iteration 6/Iteration 6 Test Cases v3 Result.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1425" windowWidth="25515" windowHeight="15540" tabRatio="674" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="4875" yWindow="1425" windowWidth="25515" windowHeight="15540" tabRatio="674" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Client -  CRUD" sheetId="17" state="hidden" r:id="rId1"/>
-    <sheet name="Login &amp; Account Management" sheetId="21" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="24" r:id="rId2"/>
     <sheet name="Screenings" sheetId="23" r:id="rId3"/>
+    <sheet name="Login &amp; Account Management" sheetId="21" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="155">
   <si>
     <t>No</t>
   </si>
@@ -682,6 +683,27 @@
       </rPr>
       <t>Regularity : 1</t>
     </r>
+  </si>
+  <si>
+    <t>Iteration 6 functions</t>
+  </si>
+  <si>
+    <t>Screening</t>
+  </si>
+  <si>
+    <t>Previous Iteration</t>
+  </si>
+  <si>
+    <t>Iter 5</t>
+  </si>
+  <si>
+    <t>Login Logout &amp; Acct Mgmt</t>
+  </si>
+  <si>
+    <t>Current Iteration: 6</t>
+  </si>
+  <si>
+    <t>RESULTS</t>
   </si>
 </sst>
 </file>
@@ -753,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -793,6 +815,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,13 +839,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3552995</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1000495</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -860,13 +883,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>106458</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2576607</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>2077171</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -904,13 +927,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3552995</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1000495</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -948,13 +971,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>106458</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2576607</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>2077171</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1520,6 +1543,623 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.875" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="3" width="39.875" customWidth="1"/>
+    <col min="4" max="4" width="57" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>21</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>25</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="88" workbookViewId="0">
@@ -3356,572 +3996,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.875" customWidth="1"/>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
-    <col min="3" max="3" width="39.875" customWidth="1"/>
-    <col min="4" max="4" width="57" customWidth="1"/>
-    <col min="5" max="5" width="23.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-    </row>
-    <row r="13" spans="1:9" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>